<commit_message>
Created alternate board designs for testing
PotSwap is for placing the potentiometer on the other side of the board,
while CapOptions allows for use of either SMD or through hole components
for resistor and capacitor.
</commit_message>
<xml_diff>
--- a/PCB Schematics/BOM.xlsx
+++ b/PCB Schematics/BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
   <si>
     <t>#ITEM</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>Per board</t>
+  </si>
+  <si>
+    <t>Lasercutting</t>
   </si>
 </sst>
 </file>
@@ -502,7 +505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -804,23 +807,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>100</v>
       </c>
       <c r="C1">
         <v>1000</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -831,7 +840,7 @@
         <v>674.42</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -842,7 +851,7 @@
         <v>206.8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -853,7 +862,7 @@
         <v>624.94000000000005</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -864,7 +873,7 @@
         <v>1483.45</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -877,7 +886,7 @@
         <v>2989.61</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
Updated BOM and silkscreen labels
For rotary encoder version of Sleep Sensei
</commit_message>
<xml_diff>
--- a/PCB Schematics/BOM.xlsx
+++ b/PCB Schematics/BOM.xlsx
@@ -13,8 +13,6 @@
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
-    <sheet name="Cost summary" sheetId="2" r:id="rId2"/>
-    <sheet name="McMaster Parts" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
   <si>
     <t>#ITEM</t>
   </si>
@@ -145,49 +143,70 @@
     <t>Standard LEDs - Through Hole Red Clear 631nm</t>
   </si>
   <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>Trimmer Resistors - Through Hole 3/8"round 10Kohms 0.5watt 20%</t>
-  </si>
-  <si>
     <t>Bourns</t>
   </si>
   <si>
-    <t>652-3352P-1-103LF</t>
-  </si>
-  <si>
-    <t>3352P-1-103LF</t>
-  </si>
-  <si>
     <t>Subtotal</t>
   </si>
   <si>
-    <t>Part #</t>
-  </si>
-  <si>
-    <t>95868A752</t>
-  </si>
-  <si>
-    <t>Nylon Socket Head Cap Screw, 1/4"-20 Thread, 2-1/2" Length, Black, packs of 100</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
-  <si>
-    <t>Units</t>
-  </si>
-  <si>
-    <t>Cost/unit</t>
-  </si>
-  <si>
-    <t>98143A011</t>
-  </si>
-  <si>
-    <t>Black Nylon 6/6 Wing Nut, 10-24 Thread Size, 29/32" Wing Spread, packs of 100</t>
-  </si>
-  <si>
-    <t>Sum</t>
+    <t>ENCODER1</t>
+  </si>
+  <si>
+    <t>VCC1</t>
+  </si>
+  <si>
+    <t>PEC12R-3220F-S0024</t>
+  </si>
+  <si>
+    <t>652-PEC12R3220FS0024</t>
+  </si>
+  <si>
+    <t>71-CRCW0201-10K</t>
+  </si>
+  <si>
+    <t>CRCW020110K0FNED</t>
+  </si>
+  <si>
+    <t>Thick Film Resistors - SMD 1/20watt 10Kohms 1% 200ppm</t>
+  </si>
+  <si>
+    <t>R6,R7</t>
+  </si>
+  <si>
+    <t>0603</t>
+  </si>
+  <si>
+    <t>0405</t>
+  </si>
+  <si>
+    <t>Encoders 20mm Shaft Switch 24 Detents 24 Pulses</t>
+  </si>
+  <si>
+    <t>12BH212A-GR</t>
+  </si>
+  <si>
+    <t>Eagle Plastic Devices</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Cylindrical Battery Contacts, Clips, Holders &amp; Springs 2 AA W/6" WIRE LDS</t>
+  </si>
+  <si>
+    <t>Knobs &amp; Dials BLK 15mm D-SHAFT</t>
+  </si>
+  <si>
+    <t>450-AA150</t>
+  </si>
+  <si>
+    <t>ATtiny85-20PU</t>
+  </si>
+  <si>
+    <t>Atmel</t>
+  </si>
+  <si>
+    <t>556-ATTINY85-20PU</t>
   </si>
 </sst>
 </file>
@@ -226,10 +245,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,16 +530,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="62.28515625" customWidth="1"/>
+    <col min="2" max="2" width="66.85546875" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="32.140625" customWidth="1"/>
@@ -566,7 +586,7 @@
         <v>29</v>
       </c>
       <c r="L1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -604,7 +624,7 @@
         <v>8.6999999999999994E-2</v>
       </c>
       <c r="L2" s="1">
-        <f t="shared" ref="L2:L6" si="0">K2*J2</f>
+        <f t="shared" ref="L2:L7" si="0">K2*J2</f>
         <v>87</v>
       </c>
     </row>
@@ -618,8 +638,8 @@
       <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="D3">
-        <v>405</v>
+      <c r="D3" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="E3" t="s">
         <v>21</v>
@@ -657,8 +677,8 @@
       <c r="C4" t="s">
         <v>23</v>
       </c>
-      <c r="D4">
-        <v>603</v>
+      <c r="D4" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="E4" t="s">
         <v>25</v>
@@ -690,39 +710,39 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>33</v>
+      <c r="B5" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>32</v>
+        <v>48</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J5">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="K5" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -730,38 +750,38 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>34</v>
+      <c r="H6" t="s">
+        <v>28</v>
       </c>
       <c r="I6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J6">
-        <v>4000</v>
+        <v>1000</v>
       </c>
       <c r="K6" s="1">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="0"/>
-        <v>240</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -769,144 +789,195 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
         <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="G7" t="s">
         <v>11</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
+      </c>
+      <c r="J7">
+        <v>4000</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="L7" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1000</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0.60399999999999998</v>
+      </c>
+      <c r="L8" s="1">
+        <f>K8*J8</f>
+        <v>604</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
         <v>42</v>
       </c>
-      <c r="I7">
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9">
         <v>1</v>
       </c>
-      <c r="J7">
+      <c r="J9">
         <v>1000</v>
       </c>
-      <c r="K7" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="L7" s="1">
-        <f>K7*J7</f>
-        <v>800</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K9" s="1"/>
+      <c r="K9" s="1">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="L9" s="1">
+        <f>K9*J9</f>
+        <v>259</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" t="s">
+        <v>57</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1000</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="L11" s="1">
+        <f>K11*J11</f>
+        <v>204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" t="s">
+        <v>60</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1000</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="L12" s="1">
+        <f>K12*J12</f>
+        <v>791</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="A1:E12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="80" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="1">
-        <v>13.2</v>
-      </c>
-      <c r="D2">
-        <v>100</v>
-      </c>
-      <c r="E2" s="1">
-        <f>C2/D2</f>
-        <v>0.13200000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="1">
-        <v>12.29</v>
-      </c>
-      <c r="D3">
-        <v>100</v>
-      </c>
-      <c r="E3" s="1">
-        <f>C3/D3</f>
-        <v>0.1229</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="1">
-        <f>E3+E2</f>
-        <v>0.25490000000000002</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated files for latest order
</commit_message>
<xml_diff>
--- a/PCB Schematics/BOM.xlsx
+++ b/PCB Schematics/BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="61">
   <si>
     <t>#ITEM</t>
   </si>
@@ -530,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,7 +551,7 @@
     <col min="11" max="11" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -588,8 +588,14 @@
       <c r="L1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -627,8 +633,15 @@
         <f t="shared" ref="L2:L7" si="0">K2*J2</f>
         <v>87</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N2">
+        <f>J2/10</f>
+        <v>100</v>
+      </c>
+      <c r="O2">
+        <v>0.127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -666,8 +679,15 @@
         <f t="shared" si="0"/>
         <v>73</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N3">
+        <f t="shared" ref="N3:N12" si="1">J3/10</f>
+        <v>100</v>
+      </c>
+      <c r="O3">
+        <v>9.4E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -705,8 +725,15 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="O4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -744,8 +771,15 @@
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N5">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="O5">
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -783,8 +817,15 @@
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="O6">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -822,8 +863,15 @@
         <f t="shared" si="0"/>
         <v>240</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+      <c r="O7">
+        <v>7.8E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -861,8 +909,15 @@
         <f>K8*J8</f>
         <v>604</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N8">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="O8">
+        <v>0.66900000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -900,8 +955,15 @@
         <f>K9*J9</f>
         <v>259</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N9">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="O9">
+        <v>0.32700000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -936,8 +998,15 @@
         <f>K11*J11</f>
         <v>204</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N11">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="O11">
+        <v>0.24399999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -975,6 +1044,26 @@
         <f>K12*J12</f>
         <v>791</v>
       </c>
+      <c r="N12">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="O12">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K14">
+        <f>SUM(K2:K12)</f>
+        <v>2.1880000000000002</v>
+      </c>
+      <c r="O14">
+        <f>SUM(O2:O12)</f>
+        <v>2.6310000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>